<commit_message>
Erro no desempate Geral
</commit_message>
<xml_diff>
--- a/prof.xlsx
+++ b/prof.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEDUC\Documents\Py\Algoritmo-lotacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E00FBAE-9A08-434E-831A-3E8AE0E5DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3B495B-6F9C-4876-850B-2514A403F5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="80">
   <si>
     <t>01A URE - BRAGANCA</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>TURNO_N_APTO</t>
+  </si>
+  <si>
+    <t>TURNO_CONCENTRADO</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DATA_</t>
   </si>
 </sst>
 </file>
@@ -628,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC31"/>
+  <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,11 +658,12 @@
     <col min="9" max="9" width="13.21875" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" customWidth="1"/>
     <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" customWidth="1"/>
-    <col min="25" max="29" width="13.5546875" customWidth="1"/>
+    <col min="16" max="16" width="10.5546875" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" customWidth="1"/>
+    <col min="27" max="31" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -694,49 +710,55 @@
         <v>9</v>
       </c>
       <c r="P1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>56</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>74</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -779,44 +801,50 @@
       <c r="O2" s="2">
         <v>44148</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P2" s="2">
+        <v>44513</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2">
+      <c r="S2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2">
         <v>2023</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>5</v>
       </c>
-      <c r="U2">
-        <v>4</v>
-      </c>
       <c r="V2">
+        <v>4</v>
+      </c>
+      <c r="W2">
         <v>44</v>
       </c>
-      <c r="W2" t="s">
-        <v>11</v>
-      </c>
       <c r="X2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2">
-        <v>1</v>
-      </c>
-      <c r="Z2">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>76</v>
       </c>
       <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -859,44 +887,50 @@
       <c r="O3" s="2">
         <v>44156</v>
       </c>
-      <c r="P3">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>2</v>
+      <c r="P3" s="2">
+        <v>44541</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3">
         <v>2023</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>5</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>5</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>40</v>
       </c>
-      <c r="W3" t="s">
-        <v>39</v>
-      </c>
       <c r="X3" t="s">
         <v>39</v>
       </c>
-      <c r="Y3">
-        <v>2</v>
-      </c>
-      <c r="Z3">
-        <v>3</v>
+      <c r="Y3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>77</v>
       </c>
       <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AC3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -939,44 +973,50 @@
       <c r="O4" s="2">
         <v>44153</v>
       </c>
-      <c r="P4">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>2</v>
+      <c r="P4" s="2">
+        <v>44542</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4">
         <v>2023</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>5</v>
       </c>
-      <c r="U4">
-        <v>4</v>
-      </c>
       <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4">
         <v>40</v>
       </c>
-      <c r="W4" t="s">
-        <v>11</v>
-      </c>
       <c r="X4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>76</v>
       </c>
       <c r="AA4">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1019,44 +1059,50 @@
       <c r="O5" s="2">
         <v>44151</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>4</v>
+      <c r="P5" s="2">
+        <v>44524</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
       </c>
       <c r="R5" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5">
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5">
         <v>2023</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>5</v>
       </c>
-      <c r="U5">
-        <v>3</v>
-      </c>
       <c r="V5">
-        <v>39</v>
-      </c>
-      <c r="W5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5">
         <v>39</v>
       </c>
       <c r="X5" t="s">
         <v>39</v>
       </c>
-      <c r="Y5">
-        <v>4</v>
-      </c>
-      <c r="Z5">
-        <v>3</v>
+      <c r="Y5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>77</v>
       </c>
       <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1099,44 +1145,50 @@
       <c r="O6" s="2">
         <v>44152</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>4</v>
+      <c r="P6" s="2">
+        <v>44525</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6">
         <v>2023</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>5</v>
       </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
       <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6">
         <v>18</v>
       </c>
-      <c r="W6" t="s">
-        <v>11</v>
-      </c>
       <c r="X6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y6">
-        <v>4</v>
-      </c>
-      <c r="Z6">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>76</v>
       </c>
       <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1179,44 +1231,53 @@
       <c r="O7" s="2">
         <v>44153</v>
       </c>
-      <c r="P7">
-        <v>3</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>2</v>
+      <c r="P7" s="2">
+        <v>44535</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
-      </c>
-      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7">
         <v>2023</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>5</v>
       </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
       <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
         <v>42</v>
       </c>
-      <c r="W7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y7">
-        <v>1</v>
-      </c>
-      <c r="Z7">
-        <v>2</v>
+      <c r="X7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>77</v>
       </c>
       <c r="AA7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AD7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1259,42 +1320,51 @@
       <c r="O8" s="2">
         <v>44150</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>4</v>
+      <c r="P8" s="2">
+        <v>44523</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>11</v>
-      </c>
-      <c r="S8">
+        <v>4</v>
+      </c>
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8">
         <v>2023</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>5</v>
       </c>
-      <c r="U8">
-        <v>3</v>
-      </c>
       <c r="V8">
-        <v>39</v>
-      </c>
-      <c r="W8" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y8">
-        <v>2</v>
-      </c>
-      <c r="Z8">
-        <v>4</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>39</v>
+      </c>
+      <c r="X8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="5"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1337,47 +1407,56 @@
       <c r="O9" s="2">
         <v>44155</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>4</v>
+      <c r="P9" s="2">
+        <v>44520</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9">
         <v>2023</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>5</v>
       </c>
-      <c r="U9">
-        <v>3</v>
-      </c>
       <c r="V9">
-        <v>39</v>
-      </c>
-      <c r="W9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <v>39</v>
+      </c>
+      <c r="X9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA9">
         <v>5</v>
       </c>
-      <c r="Z9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <v>3</v>
-      </c>
       <c r="AB9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC9">
+        <v>3</v>
+      </c>
+      <c r="AD9">
+        <v>2</v>
+      </c>
+      <c r="AE9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1420,47 +1499,56 @@
       <c r="O10" s="2">
         <v>44146</v>
       </c>
-      <c r="P10">
-        <v>3</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>2</v>
+      <c r="P10" s="2">
+        <v>44521</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
       </c>
       <c r="R10" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="S10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10">
         <v>2023</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>5</v>
       </c>
-      <c r="U10">
-        <v>3</v>
-      </c>
       <c r="V10">
+        <v>3</v>
+      </c>
+      <c r="W10">
         <v>33</v>
       </c>
-      <c r="W10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y10">
-        <v>1</v>
-      </c>
-      <c r="Z10">
-        <v>2</v>
+      <c r="X10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>76</v>
       </c>
       <c r="AA10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC10">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1503,44 +1591,53 @@
       <c r="O11" s="2">
         <v>44152</v>
       </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>4</v>
+      <c r="P11" s="2">
+        <v>44522</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>11</v>
-      </c>
-      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="S11" t="s">
+        <v>11</v>
+      </c>
+      <c r="T11">
         <v>2023</v>
       </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
         <v>5</v>
       </c>
-      <c r="U11">
-        <v>3</v>
-      </c>
       <c r="V11">
-        <v>39</v>
-      </c>
-      <c r="W11" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y11">
-        <v>4</v>
-      </c>
-      <c r="Z11">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="W11">
+        <v>39</v>
+      </c>
+      <c r="X11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>76</v>
       </c>
       <c r="AA11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1583,41 +1680,50 @@
       <c r="O12" s="2">
         <v>44148</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="P12" s="2">
+        <v>44523</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
         <v>7</v>
       </c>
-      <c r="R12" t="s">
-        <v>11</v>
-      </c>
-      <c r="S12">
+      <c r="S12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12">
         <v>2023</v>
       </c>
-      <c r="T12" t="s">
-        <v>3</v>
-      </c>
-      <c r="U12">
-        <v>4</v>
+      <c r="U12" t="s">
+        <v>3</v>
       </c>
       <c r="V12">
+        <v>4</v>
+      </c>
+      <c r="W12">
         <v>44</v>
       </c>
-      <c r="W12" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
-      <c r="Z12">
-        <v>2</v>
+      <c r="X12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>76</v>
       </c>
       <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
+      </c>
+      <c r="AC12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1660,41 +1766,50 @@
       <c r="O13" s="2">
         <v>44156</v>
       </c>
-      <c r="P13">
-        <v>3</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>2</v>
+      <c r="P13" s="2">
+        <v>44541</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
       </c>
       <c r="R13" t="s">
-        <v>39</v>
-      </c>
-      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="S13" t="s">
+        <v>39</v>
+      </c>
+      <c r="T13">
         <v>2023</v>
       </c>
-      <c r="T13" t="s">
-        <v>3</v>
-      </c>
-      <c r="U13">
+      <c r="U13" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13">
         <v>5</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>40</v>
       </c>
-      <c r="W13" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y13">
-        <v>2</v>
-      </c>
-      <c r="Z13">
-        <v>3</v>
+      <c r="X13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>77</v>
       </c>
       <c r="AA13">
+        <v>2</v>
+      </c>
+      <c r="AB13">
+        <v>3</v>
+      </c>
+      <c r="AC13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1737,41 +1852,50 @@
       <c r="O14" s="2">
         <v>44153</v>
       </c>
-      <c r="P14">
-        <v>3</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>2</v>
+      <c r="P14" s="2">
+        <v>44542</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
       </c>
       <c r="R14" t="s">
-        <v>11</v>
-      </c>
-      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="S14" t="s">
+        <v>11</v>
+      </c>
+      <c r="T14">
         <v>2023</v>
       </c>
-      <c r="T14" t="s">
-        <v>3</v>
-      </c>
-      <c r="U14">
-        <v>4</v>
+      <c r="U14" t="s">
+        <v>3</v>
       </c>
       <c r="V14">
+        <v>4</v>
+      </c>
+      <c r="W14">
         <v>40</v>
       </c>
-      <c r="W14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y14">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="5">
-        <v>1</v>
+      <c r="X14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>78</v>
       </c>
       <c r="AA14">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1814,41 +1938,50 @@
       <c r="O15" s="2">
         <v>44151</v>
       </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>4</v>
+      <c r="P15" s="2">
+        <v>44526</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>39</v>
-      </c>
-      <c r="S15">
+        <v>4</v>
+      </c>
+      <c r="S15" t="s">
+        <v>39</v>
+      </c>
+      <c r="T15">
         <v>2023</v>
       </c>
-      <c r="T15" t="s">
-        <v>3</v>
-      </c>
-      <c r="U15">
+      <c r="U15" t="s">
         <v>3</v>
       </c>
       <c r="V15">
-        <v>39</v>
-      </c>
-      <c r="W15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y15">
-        <v>4</v>
-      </c>
-      <c r="Z15">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <v>39</v>
+      </c>
+      <c r="X15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>77</v>
       </c>
       <c r="AA15">
+        <v>4</v>
+      </c>
+      <c r="AB15">
+        <v>3</v>
+      </c>
+      <c r="AC15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1891,41 +2024,50 @@
       <c r="O16" s="2">
         <v>44152</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>4</v>
+      <c r="P16" s="2">
+        <v>44527</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>11</v>
-      </c>
-      <c r="S16">
+        <v>4</v>
+      </c>
+      <c r="S16" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16">
         <v>2023</v>
       </c>
-      <c r="T16" t="s">
-        <v>3</v>
-      </c>
-      <c r="U16">
+      <c r="U16" t="s">
         <v>3</v>
       </c>
       <c r="V16">
+        <v>3</v>
+      </c>
+      <c r="W16">
         <v>18</v>
       </c>
-      <c r="W16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y16">
-        <v>4</v>
-      </c>
-      <c r="Z16">
-        <v>2</v>
+      <c r="X16" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>78</v>
       </c>
       <c r="AA16">
+        <v>4</v>
+      </c>
+      <c r="AB16">
+        <v>2</v>
+      </c>
+      <c r="AC16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1968,44 +2110,53 @@
       <c r="O17" s="2">
         <v>44153</v>
       </c>
-      <c r="P17">
-        <v>3</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>2</v>
+      <c r="P17" s="2">
+        <v>44537</v>
+      </c>
+      <c r="Q17">
+        <v>3</v>
       </c>
       <c r="R17" t="s">
-        <v>39</v>
-      </c>
-      <c r="S17">
+        <v>2</v>
+      </c>
+      <c r="S17" t="s">
+        <v>39</v>
+      </c>
+      <c r="T17">
         <v>2023</v>
       </c>
-      <c r="T17" t="s">
-        <v>3</v>
-      </c>
-      <c r="U17">
+      <c r="U17" t="s">
         <v>3</v>
       </c>
       <c r="V17">
+        <v>3</v>
+      </c>
+      <c r="W17">
         <v>42</v>
       </c>
-      <c r="W17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
-      <c r="Z17">
-        <v>2</v>
+      <c r="X17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>76</v>
       </c>
       <c r="AA17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB17">
+        <v>2</v>
+      </c>
+      <c r="AC17">
+        <v>3</v>
+      </c>
+      <c r="AD17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2048,42 +2199,51 @@
       <c r="O18" s="2">
         <v>44150</v>
       </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>4</v>
+      <c r="P18" s="2">
+        <v>44538</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>11</v>
-      </c>
-      <c r="S18">
+        <v>4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>11</v>
+      </c>
+      <c r="T18">
         <v>2023</v>
       </c>
-      <c r="T18" t="s">
-        <v>3</v>
-      </c>
-      <c r="U18">
+      <c r="U18" t="s">
         <v>3</v>
       </c>
       <c r="V18">
-        <v>39</v>
-      </c>
-      <c r="W18" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y18">
-        <v>2</v>
-      </c>
-      <c r="Z18">
-        <v>4</v>
-      </c>
-      <c r="AA18" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="W18">
+        <v>39</v>
+      </c>
+      <c r="X18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <v>4</v>
+      </c>
+      <c r="AC18" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="5"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2126,47 +2286,56 @@
       <c r="O19" s="2">
         <v>44155</v>
       </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>4</v>
+      <c r="P19" s="2">
+        <v>44524</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>39</v>
-      </c>
-      <c r="S19">
+        <v>4</v>
+      </c>
+      <c r="S19" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19">
         <v>2023</v>
       </c>
-      <c r="T19" t="s">
-        <v>3</v>
-      </c>
-      <c r="U19">
+      <c r="U19" t="s">
         <v>3</v>
       </c>
       <c r="V19">
-        <v>39</v>
-      </c>
-      <c r="W19" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y19">
+        <v>3</v>
+      </c>
+      <c r="W19">
+        <v>39</v>
+      </c>
+      <c r="X19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA19">
         <v>5</v>
       </c>
-      <c r="Z19">
-        <v>1</v>
-      </c>
-      <c r="AA19">
-        <v>3</v>
-      </c>
       <c r="AB19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC19">
+        <v>3</v>
+      </c>
+      <c r="AD19">
+        <v>2</v>
+      </c>
+      <c r="AE19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2209,47 +2378,56 @@
       <c r="O20" s="2">
         <v>44146</v>
       </c>
-      <c r="P20">
-        <v>3</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>2</v>
+      <c r="P20" s="2">
+        <v>44525</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
       </c>
       <c r="R20" t="s">
-        <v>11</v>
-      </c>
-      <c r="S20">
+        <v>2</v>
+      </c>
+      <c r="S20" t="s">
+        <v>11</v>
+      </c>
+      <c r="T20">
         <v>2023</v>
       </c>
-      <c r="T20" t="s">
-        <v>3</v>
-      </c>
-      <c r="U20">
+      <c r="U20" t="s">
         <v>3</v>
       </c>
       <c r="V20">
+        <v>3</v>
+      </c>
+      <c r="W20">
         <v>33</v>
       </c>
-      <c r="W20" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y20">
-        <v>1</v>
-      </c>
-      <c r="Z20">
-        <v>2</v>
+      <c r="X20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>77</v>
       </c>
       <c r="AA20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC20">
+        <v>3</v>
+      </c>
+      <c r="AD20">
+        <v>4</v>
+      </c>
+      <c r="AE20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2292,44 +2470,53 @@
       <c r="O21" s="2">
         <v>44152</v>
       </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>4</v>
+      <c r="P21" s="2">
+        <v>44526</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>11</v>
-      </c>
-      <c r="S21">
+        <v>4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>11</v>
+      </c>
+      <c r="T21">
         <v>2023</v>
       </c>
-      <c r="T21" t="s">
-        <v>3</v>
-      </c>
-      <c r="U21">
+      <c r="U21" t="s">
         <v>3</v>
       </c>
       <c r="V21">
-        <v>39</v>
-      </c>
-      <c r="W21" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y21">
-        <v>4</v>
-      </c>
-      <c r="Z21">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="W21">
+        <v>39</v>
+      </c>
+      <c r="X21" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>76</v>
       </c>
       <c r="AA21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB21">
+        <v>3</v>
+      </c>
+      <c r="AC21">
+        <v>2</v>
+      </c>
+      <c r="AD21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2372,41 +2559,50 @@
       <c r="O22" s="2">
         <v>44148</v>
       </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="P22" s="2">
+        <v>44523</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
         <v>7</v>
       </c>
-      <c r="R22" t="s">
-        <v>11</v>
-      </c>
-      <c r="S22">
+      <c r="S22" t="s">
+        <v>11</v>
+      </c>
+      <c r="T22">
         <v>2023</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>40</v>
       </c>
-      <c r="U22">
-        <v>4</v>
-      </c>
       <c r="V22">
+        <v>4</v>
+      </c>
+      <c r="W22">
         <v>44</v>
       </c>
-      <c r="W22" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y22">
-        <v>1</v>
-      </c>
-      <c r="Z22">
-        <v>2</v>
+      <c r="X22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>76</v>
       </c>
       <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>2</v>
+      </c>
+      <c r="AC22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2449,41 +2645,50 @@
       <c r="O23" s="2">
         <v>44156</v>
       </c>
-      <c r="P23">
-        <v>3</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>2</v>
+      <c r="P23" s="2">
+        <v>44536</v>
+      </c>
+      <c r="Q23">
+        <v>3</v>
       </c>
       <c r="R23" t="s">
-        <v>39</v>
-      </c>
-      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="S23" t="s">
+        <v>39</v>
+      </c>
+      <c r="T23">
         <v>2023</v>
       </c>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>40</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>5</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>40</v>
       </c>
-      <c r="W23" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y23">
-        <v>2</v>
-      </c>
-      <c r="Z23">
-        <v>3</v>
+      <c r="X23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>77</v>
       </c>
       <c r="AA23">
+        <v>2</v>
+      </c>
+      <c r="AB23">
+        <v>3</v>
+      </c>
+      <c r="AC23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2526,41 +2731,50 @@
       <c r="O24" s="2">
         <v>44153</v>
       </c>
-      <c r="P24">
-        <v>3</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>2</v>
+      <c r="P24" s="2">
+        <v>44535</v>
+      </c>
+      <c r="Q24">
+        <v>3</v>
       </c>
       <c r="R24" t="s">
-        <v>11</v>
-      </c>
-      <c r="S24">
+        <v>2</v>
+      </c>
+      <c r="S24" t="s">
+        <v>11</v>
+      </c>
+      <c r="T24">
         <v>2023</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>40</v>
       </c>
-      <c r="U24">
-        <v>4</v>
-      </c>
       <c r="V24">
+        <v>4</v>
+      </c>
+      <c r="W24">
         <v>40</v>
       </c>
-      <c r="W24" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y24">
-        <v>3</v>
-      </c>
-      <c r="Z24" s="5">
-        <v>1</v>
+      <c r="X24" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>78</v>
       </c>
       <c r="AA24">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2603,41 +2817,50 @@
       <c r="O25" s="2">
         <v>44151</v>
       </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>4</v>
+      <c r="P25" s="2">
+        <v>44536</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>39</v>
-      </c>
-      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="S25" t="s">
+        <v>39</v>
+      </c>
+      <c r="T25">
         <v>2023</v>
       </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>40</v>
       </c>
-      <c r="U25">
-        <v>3</v>
-      </c>
       <c r="V25">
-        <v>39</v>
-      </c>
-      <c r="W25" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y25">
-        <v>4</v>
-      </c>
-      <c r="Z25">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="W25">
+        <v>39</v>
+      </c>
+      <c r="X25" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>77</v>
       </c>
       <c r="AA25">
+        <v>4</v>
+      </c>
+      <c r="AB25">
+        <v>3</v>
+      </c>
+      <c r="AC25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2680,41 +2903,50 @@
       <c r="O26" s="2">
         <v>44152</v>
       </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>4</v>
+      <c r="P26" s="2">
+        <v>44537</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>11</v>
-      </c>
-      <c r="S26">
+        <v>4</v>
+      </c>
+      <c r="S26" t="s">
+        <v>11</v>
+      </c>
+      <c r="T26">
         <v>2023</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>40</v>
       </c>
-      <c r="U26">
-        <v>3</v>
-      </c>
       <c r="V26">
+        <v>3</v>
+      </c>
+      <c r="W26">
         <v>18</v>
       </c>
-      <c r="W26" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y26">
-        <v>4</v>
-      </c>
-      <c r="Z26">
-        <v>2</v>
+      <c r="X26" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>77</v>
       </c>
       <c r="AA26">
+        <v>4</v>
+      </c>
+      <c r="AB26">
+        <v>2</v>
+      </c>
+      <c r="AC26">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2757,44 +2989,53 @@
       <c r="O27" s="2">
         <v>44153</v>
       </c>
-      <c r="P27">
-        <v>3</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>2</v>
+      <c r="P27" s="2">
+        <v>44538</v>
+      </c>
+      <c r="Q27">
+        <v>3</v>
       </c>
       <c r="R27" t="s">
-        <v>39</v>
-      </c>
-      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="S27" t="s">
+        <v>39</v>
+      </c>
+      <c r="T27">
         <v>2023</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>40</v>
       </c>
-      <c r="U27">
-        <v>3</v>
-      </c>
       <c r="V27">
+        <v>3</v>
+      </c>
+      <c r="W27">
         <v>42</v>
       </c>
-      <c r="W27" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-      <c r="Z27">
-        <v>2</v>
+      <c r="X27" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>76</v>
       </c>
       <c r="AA27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB27">
+        <v>2</v>
+      </c>
+      <c r="AC27">
+        <v>3</v>
+      </c>
+      <c r="AD27">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2837,42 +3078,51 @@
       <c r="O28" s="2">
         <v>44150</v>
       </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>4</v>
+      <c r="P28" s="2">
+        <v>44539</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
       </c>
       <c r="R28" t="s">
-        <v>11</v>
-      </c>
-      <c r="S28">
+        <v>4</v>
+      </c>
+      <c r="S28" t="s">
+        <v>11</v>
+      </c>
+      <c r="T28">
         <v>2023</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>40</v>
       </c>
-      <c r="U28">
-        <v>3</v>
-      </c>
       <c r="V28">
-        <v>39</v>
-      </c>
-      <c r="W28" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y28">
-        <v>2</v>
-      </c>
-      <c r="Z28">
-        <v>4</v>
-      </c>
-      <c r="AA28" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC28" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="W28">
+        <v>39</v>
+      </c>
+      <c r="X28" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA28">
+        <v>2</v>
+      </c>
+      <c r="AB28">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="5"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2915,47 +3165,56 @@
       <c r="O29" s="2">
         <v>44155</v>
       </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>4</v>
+      <c r="P29" s="2">
+        <v>44540</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
       </c>
       <c r="R29" t="s">
-        <v>39</v>
-      </c>
-      <c r="S29">
+        <v>4</v>
+      </c>
+      <c r="S29" t="s">
+        <v>39</v>
+      </c>
+      <c r="T29">
         <v>2023</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
         <v>40</v>
       </c>
-      <c r="U29">
-        <v>3</v>
-      </c>
       <c r="V29">
-        <v>39</v>
-      </c>
-      <c r="W29" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y29">
+        <v>3</v>
+      </c>
+      <c r="W29">
+        <v>39</v>
+      </c>
+      <c r="X29" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA29">
         <v>5</v>
       </c>
-      <c r="Z29">
-        <v>1</v>
-      </c>
-      <c r="AA29">
-        <v>3</v>
-      </c>
       <c r="AB29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC29">
+        <v>3</v>
+      </c>
+      <c r="AD29">
+        <v>2</v>
+      </c>
+      <c r="AE29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2998,47 +3257,56 @@
       <c r="O30" s="2">
         <v>44146</v>
       </c>
-      <c r="P30">
-        <v>3</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>2</v>
+      <c r="P30" s="2">
+        <v>44541</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
       </c>
       <c r="R30" t="s">
-        <v>11</v>
-      </c>
-      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="S30" t="s">
+        <v>11</v>
+      </c>
+      <c r="T30">
         <v>2023</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>40</v>
       </c>
-      <c r="U30">
-        <v>3</v>
-      </c>
       <c r="V30">
+        <v>3</v>
+      </c>
+      <c r="W30">
         <v>33</v>
       </c>
-      <c r="W30" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y30">
-        <v>1</v>
-      </c>
-      <c r="Z30">
-        <v>2</v>
+      <c r="X30" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>77</v>
       </c>
       <c r="AA30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC30">
+        <v>3</v>
+      </c>
+      <c r="AD30">
+        <v>4</v>
+      </c>
+      <c r="AE30">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -3081,45 +3349,54 @@
       <c r="O31" s="2">
         <v>44152</v>
       </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>4</v>
+      <c r="P31" s="2">
+        <v>44542</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
       </c>
       <c r="R31" t="s">
-        <v>11</v>
-      </c>
-      <c r="S31">
+        <v>4</v>
+      </c>
+      <c r="S31" t="s">
+        <v>11</v>
+      </c>
+      <c r="T31">
         <v>2023</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>40</v>
       </c>
-      <c r="U31">
-        <v>3</v>
-      </c>
       <c r="V31">
-        <v>39</v>
-      </c>
-      <c r="W31" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y31">
-        <v>4</v>
-      </c>
-      <c r="Z31">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="W31">
+        <v>39</v>
+      </c>
+      <c r="X31" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>78</v>
       </c>
       <c r="AA31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AB31">
+        <v>3</v>
+      </c>
+      <c r="AC31">
+        <v>2</v>
+      </c>
+      <c r="AD31">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AE11" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>